<commit_message>
both pages and sidebar
</commit_message>
<xml_diff>
--- a/data/processed/ABS_v1_report.xlsx
+++ b/data/processed/ABS_v1_report.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">F-REQ-001</t>
   </si>
   <si>
-    <t xml:space="preserve">PASSED</t>
+    <t xml:space="preserve">Passed</t>
   </si>
   <si>
     <t xml:space="preserve">F-REQ-002</t>
@@ -40,7 +40,7 @@
     <t xml:space="preserve">F-REQ-003</t>
   </si>
   <si>
-    <t xml:space="preserve">FAILED</t>
+    <t xml:space="preserve">Failed</t>
   </si>
   <si>
     <t xml:space="preserve">F-REQ-004</t>
@@ -91,7 +91,7 @@
     <t xml:space="preserve">F-REQ-019</t>
   </si>
   <si>
-    <t xml:space="preserve">Not_applicable</t>
+    <t xml:space="preserve">Not_Applicable</t>
   </si>
   <si>
     <t xml:space="preserve">F-REQ-020</t>
@@ -244,11 +244,11 @@
   </sheetPr>
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.39"/>

</xml_diff>